<commit_message>
Updated for U13C Leucine Study
</commit_message>
<xml_diff>
--- a/molecules-lists/1- USE THIS TO CREATE LISTS.xlsx
+++ b/molecules-lists/1- USE THIS TO CREATE LISTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\2020_Scripts for Data Processing\Git Repository (March 2020)\molecules-lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA6DC7C-FCFB-492B-877E-2E78DA17E7D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CC19A7-0013-4C0A-AA08-7FE54B51E9D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DA222FD2-02EA-429D-8431-AFA8895842CE}"/>
   </bookViews>
@@ -94,8 +94,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000000000"/>
-    <numFmt numFmtId="169" formatCode="0.000000000"/>
-    <numFmt numFmtId="173" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -712,8 +712,8 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1425,7 +1425,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T15" sqref="T15"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1452,16 +1452,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>12</v>
@@ -1499,7 +1499,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="11">
-        <f>(B2*$Q$2)+(C2*$Q$3)+(D2*$Q$4)+(E2*$Q$5)+(F2*$Q$6)+(G2*$Q$7)+(H2*$Q$8)+(I2*$Q$9)+(J2*$Q$10)+(K2*$Q$11)+(L2*$Q$12)</f>
+        <f>(B2*$Q$2)+(C2*$Q$3)+(D2*$Q$4)+(F2*$Q$5)+(G2*$Q$6)+(H2*$Q$7)+(E2*$Q$8)+(I2*$Q$9)+(J2*$Q$10)+(K2*$Q$11)+(L2*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P2" s="7" t="s">
@@ -1514,7 +1514,7 @@
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="M3" s="11">
-        <f t="shared" ref="M3:M31" si="0">(B3*$Q$2)+(C3*$Q$3)+(D3*$Q$4)+(E3*$Q$5)+(F3*$Q$6)+(G3*$Q$7)+(H3*$Q$8)+(I3*$Q$9)+(J3*$Q$10)+(K3*$Q$11)+(L3*$Q$12)</f>
+        <f>(B3*$Q$2)+(C3*$Q$3)+(D3*$Q$4)+(F3*$Q$5)+(G3*$Q$6)+(H3*$Q$7)+(E3*$Q$8)+(I3*$Q$9)+(J3*$Q$10)+(K3*$Q$11)+(L3*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P3" s="7" t="s">
@@ -1529,7 +1529,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="M4" s="11">
-        <f t="shared" si="0"/>
+        <f>(B4*$Q$2)+(C4*$Q$3)+(D4*$Q$4)+(F4*$Q$5)+(G4*$Q$6)+(H4*$Q$7)+(E4*$Q$8)+(I4*$Q$9)+(J4*$Q$10)+(K4*$Q$11)+(L4*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P4" s="7" t="s">
@@ -1544,7 +1544,7 @@
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="M5" s="11">
-        <f t="shared" si="0"/>
+        <f>(B5*$Q$2)+(C5*$Q$3)+(D5*$Q$4)+(F5*$Q$5)+(G5*$Q$6)+(H5*$Q$7)+(E5*$Q$8)+(I5*$Q$9)+(J5*$Q$10)+(K5*$Q$11)+(L5*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P5" s="7" t="s">
@@ -1559,7 +1559,7 @@
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="M6" s="11">
-        <f t="shared" si="0"/>
+        <f>(B6*$Q$2)+(C6*$Q$3)+(D6*$Q$4)+(F6*$Q$5)+(G6*$Q$6)+(H6*$Q$7)+(E6*$Q$8)+(I6*$Q$9)+(J6*$Q$10)+(K6*$Q$11)+(L6*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P6" s="7" t="s">
@@ -1574,7 +1574,7 @@
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="M7" s="11">
-        <f t="shared" si="0"/>
+        <f>(B7*$Q$2)+(C7*$Q$3)+(D7*$Q$4)+(F7*$Q$5)+(G7*$Q$6)+(H7*$Q$7)+(E7*$Q$8)+(I7*$Q$9)+(J7*$Q$10)+(K7*$Q$11)+(L7*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P7" s="7" t="s">
@@ -1589,7 +1589,7 @@
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
       <c r="M8" s="11">
-        <f t="shared" si="0"/>
+        <f>(B8*$Q$2)+(C8*$Q$3)+(D8*$Q$4)+(F8*$Q$5)+(G8*$Q$6)+(H8*$Q$7)+(E8*$Q$8)+(I8*$Q$9)+(J8*$Q$10)+(K8*$Q$11)+(L8*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P8" s="7" t="s">
@@ -1604,7 +1604,7 @@
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="M9" s="11">
-        <f t="shared" si="0"/>
+        <f>(B9*$Q$2)+(C9*$Q$3)+(D9*$Q$4)+(F9*$Q$5)+(G9*$Q$6)+(H9*$Q$7)+(E9*$Q$8)+(I9*$Q$9)+(J9*$Q$10)+(K9*$Q$11)+(L9*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P9" s="7" t="s">
@@ -1619,7 +1619,7 @@
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
       <c r="M10" s="11">
-        <f t="shared" si="0"/>
+        <f>(B10*$Q$2)+(C10*$Q$3)+(D10*$Q$4)+(F10*$Q$5)+(G10*$Q$6)+(H10*$Q$7)+(E10*$Q$8)+(I10*$Q$9)+(J10*$Q$10)+(K10*$Q$11)+(L10*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P10" s="7" t="s">
@@ -1634,7 +1634,7 @@
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="M11" s="11">
-        <f t="shared" si="0"/>
+        <f>(B11*$Q$2)+(C11*$Q$3)+(D11*$Q$4)+(F11*$Q$5)+(G11*$Q$6)+(H11*$Q$7)+(E11*$Q$8)+(I11*$Q$9)+(J11*$Q$10)+(K11*$Q$11)+(L11*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P11" s="7" t="s">
@@ -1649,7 +1649,7 @@
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="M12" s="11">
-        <f t="shared" si="0"/>
+        <f>(B12*$Q$2)+(C12*$Q$3)+(D12*$Q$4)+(F12*$Q$5)+(G12*$Q$6)+(H12*$Q$7)+(E12*$Q$8)+(I12*$Q$9)+(J12*$Q$10)+(K12*$Q$11)+(L12*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P12" s="7" t="s">
@@ -1664,7 +1664,7 @@
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="M13" s="11">
-        <f t="shared" si="0"/>
+        <f>(B13*$Q$2)+(C13*$Q$3)+(D13*$Q$4)+(F13*$Q$5)+(G13*$Q$6)+(H13*$Q$7)+(E13*$Q$8)+(I13*$Q$9)+(J13*$Q$10)+(K13*$Q$11)+(L13*$Q$12)</f>
         <v>0</v>
       </c>
     </row>
@@ -1673,7 +1673,7 @@
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="M14" s="11">
-        <f t="shared" si="0"/>
+        <f>(B14*$Q$2)+(C14*$Q$3)+(D14*$Q$4)+(F14*$Q$5)+(G14*$Q$6)+(H14*$Q$7)+(E14*$Q$8)+(I14*$Q$9)+(J14*$Q$10)+(K14*$Q$11)+(L14*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P14" s="19" t="s">
@@ -1688,7 +1688,7 @@
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="M15" s="11">
-        <f t="shared" si="0"/>
+        <f>(B15*$Q$2)+(C15*$Q$3)+(D15*$Q$4)+(F15*$Q$5)+(G15*$Q$6)+(H15*$Q$7)+(E15*$Q$8)+(I15*$Q$9)+(J15*$Q$10)+(K15*$Q$11)+(L15*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P15" s="22"/>
@@ -1701,7 +1701,7 @@
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="M16" s="11">
-        <f t="shared" si="0"/>
+        <f>(B16*$Q$2)+(C16*$Q$3)+(D16*$Q$4)+(F16*$Q$5)+(G16*$Q$6)+(H16*$Q$7)+(E16*$Q$8)+(I16*$Q$9)+(J16*$Q$10)+(K16*$Q$11)+(L16*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P16" s="22"/>
@@ -1714,7 +1714,7 @@
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
       <c r="M17" s="11">
-        <f t="shared" si="0"/>
+        <f>(B17*$Q$2)+(C17*$Q$3)+(D17*$Q$4)+(F17*$Q$5)+(G17*$Q$6)+(H17*$Q$7)+(E17*$Q$8)+(I17*$Q$9)+(J17*$Q$10)+(K17*$Q$11)+(L17*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P17" s="22"/>
@@ -1727,7 +1727,7 @@
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
       <c r="M18" s="11">
-        <f t="shared" si="0"/>
+        <f>(B18*$Q$2)+(C18*$Q$3)+(D18*$Q$4)+(F18*$Q$5)+(G18*$Q$6)+(H18*$Q$7)+(E18*$Q$8)+(I18*$Q$9)+(J18*$Q$10)+(K18*$Q$11)+(L18*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P18" s="22"/>
@@ -1740,7 +1740,7 @@
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
       <c r="M19" s="11">
-        <f t="shared" si="0"/>
+        <f>(B19*$Q$2)+(C19*$Q$3)+(D19*$Q$4)+(F19*$Q$5)+(G19*$Q$6)+(H19*$Q$7)+(E19*$Q$8)+(I19*$Q$9)+(J19*$Q$10)+(K19*$Q$11)+(L19*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P19" s="22"/>
@@ -1753,7 +1753,7 @@
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
       <c r="M20" s="11">
-        <f t="shared" si="0"/>
+        <f>(B20*$Q$2)+(C20*$Q$3)+(D20*$Q$4)+(F20*$Q$5)+(G20*$Q$6)+(H20*$Q$7)+(E20*$Q$8)+(I20*$Q$9)+(J20*$Q$10)+(K20*$Q$11)+(L20*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P20" s="22"/>
@@ -1766,7 +1766,7 @@
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="M21" s="11">
-        <f t="shared" si="0"/>
+        <f>(B21*$Q$2)+(C21*$Q$3)+(D21*$Q$4)+(F21*$Q$5)+(G21*$Q$6)+(H21*$Q$7)+(E21*$Q$8)+(I21*$Q$9)+(J21*$Q$10)+(K21*$Q$11)+(L21*$Q$12)</f>
         <v>0</v>
       </c>
       <c r="P21" s="25"/>
@@ -1779,7 +1779,7 @@
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
       <c r="M22" s="11">
-        <f t="shared" si="0"/>
+        <f>(B22*$Q$2)+(C22*$Q$3)+(D22*$Q$4)+(F22*$Q$5)+(G22*$Q$6)+(H22*$Q$7)+(E22*$Q$8)+(I22*$Q$9)+(J22*$Q$10)+(K22*$Q$11)+(L22*$Q$12)</f>
         <v>0</v>
       </c>
     </row>
@@ -1788,7 +1788,7 @@
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
       <c r="M23" s="11">
-        <f t="shared" si="0"/>
+        <f>(B23*$Q$2)+(C23*$Q$3)+(D23*$Q$4)+(F23*$Q$5)+(G23*$Q$6)+(H23*$Q$7)+(E23*$Q$8)+(I23*$Q$9)+(J23*$Q$10)+(K23*$Q$11)+(L23*$Q$12)</f>
         <v>0</v>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
       <c r="M24" s="11">
-        <f t="shared" si="0"/>
+        <f>(B24*$Q$2)+(C24*$Q$3)+(D24*$Q$4)+(F24*$Q$5)+(G24*$Q$6)+(H24*$Q$7)+(E24*$Q$8)+(I24*$Q$9)+(J24*$Q$10)+(K24*$Q$11)+(L24*$Q$12)</f>
         <v>0</v>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
       <c r="M25" s="11">
-        <f t="shared" si="0"/>
+        <f>(B25*$Q$2)+(C25*$Q$3)+(D25*$Q$4)+(F25*$Q$5)+(G25*$Q$6)+(H25*$Q$7)+(E25*$Q$8)+(I25*$Q$9)+(J25*$Q$10)+(K25*$Q$11)+(L25*$Q$12)</f>
         <v>0</v>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
       <c r="M26" s="11">
-        <f t="shared" si="0"/>
+        <f>(B26*$Q$2)+(C26*$Q$3)+(D26*$Q$4)+(F26*$Q$5)+(G26*$Q$6)+(H26*$Q$7)+(E26*$Q$8)+(I26*$Q$9)+(J26*$Q$10)+(K26*$Q$11)+(L26*$Q$12)</f>
         <v>0</v>
       </c>
     </row>
@@ -1824,7 +1824,7 @@
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
       <c r="M27" s="11">
-        <f t="shared" si="0"/>
+        <f>(B27*$Q$2)+(C27*$Q$3)+(D27*$Q$4)+(F27*$Q$5)+(G27*$Q$6)+(H27*$Q$7)+(E27*$Q$8)+(I27*$Q$9)+(J27*$Q$10)+(K27*$Q$11)+(L27*$Q$12)</f>
         <v>0</v>
       </c>
     </row>
@@ -1833,7 +1833,7 @@
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="M28" s="11">
-        <f t="shared" si="0"/>
+        <f>(B28*$Q$2)+(C28*$Q$3)+(D28*$Q$4)+(F28*$Q$5)+(G28*$Q$6)+(H28*$Q$7)+(E28*$Q$8)+(I28*$Q$9)+(J28*$Q$10)+(K28*$Q$11)+(L28*$Q$12)</f>
         <v>0</v>
       </c>
     </row>
@@ -1842,7 +1842,7 @@
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="M29" s="11">
-        <f t="shared" si="0"/>
+        <f>(B29*$Q$2)+(C29*$Q$3)+(D29*$Q$4)+(F29*$Q$5)+(G29*$Q$6)+(H29*$Q$7)+(E29*$Q$8)+(I29*$Q$9)+(J29*$Q$10)+(K29*$Q$11)+(L29*$Q$12)</f>
         <v>0</v>
       </c>
     </row>
@@ -1851,7 +1851,7 @@
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
       <c r="M30" s="11">
-        <f t="shared" si="0"/>
+        <f>(B30*$Q$2)+(C30*$Q$3)+(D30*$Q$4)+(F30*$Q$5)+(G30*$Q$6)+(H30*$Q$7)+(E30*$Q$8)+(I30*$Q$9)+(J30*$Q$10)+(K30*$Q$11)+(L30*$Q$12)</f>
         <v>0</v>
       </c>
     </row>
@@ -1860,7 +1860,7 @@
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
       <c r="M31" s="11">
-        <f t="shared" si="0"/>
+        <f>(B31*$Q$2)+(C31*$Q$3)+(D31*$Q$4)+(F31*$Q$5)+(G31*$Q$6)+(H31*$Q$7)+(E31*$Q$8)+(I31*$Q$9)+(J31*$Q$10)+(K31*$Q$11)+(L31*$Q$12)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>